<commit_message>
Update to renv.lock and parameters.xlsx file based on enhanced flexibility incorporated into edmaps
</commit_message>
<xml_diff>
--- a/user_input/parameters.xlsx
+++ b/user_input/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcamac/Dropbox/Projects/CEBRA/edmaps/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbau/projects/tests/test-zonation-project-edmaps-1.11.0/data/user_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077B8F98-AF0D-1C4A-8DF1-7551927E4E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{500790AB-647D-584E-99CB-A0E36B687705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10020" yWindow="500" windowWidth="28380" windowHeight="21100" xr2:uid="{A299D337-5684-394D-A957-3A46518C7947}"/>
+    <workbookView xWindow="1280" yWindow="500" windowWidth="35840" windowHeight="21100" xr2:uid="{A299D337-5684-394D-A957-3A46518C7947}"/>
   </bookViews>
   <sheets>
     <sheet name="Global parameters" sheetId="7" r:id="rId1"/>
@@ -245,7 +245,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="291">
   <si>
     <t>Citrus Canker</t>
   </si>
@@ -1161,76 +1161,112 @@
     <t>Apis mellifera</t>
   </si>
   <si>
-    <t>abiotic/occurrences/gypsy_moth/cabi_Lymantria_dispar_14Dec2020.csv</t>
-  </si>
-  <si>
-    <t>abiotic/occurrences/apis_cerana/ApisCerana_DAWE.csv</t>
-  </si>
-  <si>
-    <t>abiotic/occurrences/BMSB/bmsb_presences_iprrg.csv</t>
-  </si>
-  <si>
-    <t>abiotic/occurrences/BMSB/cabi_halyomorpha halys_14Dec2020.csv</t>
-  </si>
-  <si>
-    <t>abiotic/occurrences/oriental_fruitfly/dorsalis_occurrences.csv</t>
-  </si>
-  <si>
-    <t>abiotic/occurrences/oriental_fruitfly/cabi_bactrocera_dorsalis_14Dec2020.csv</t>
-  </si>
-  <si>
-    <t>abiotic/occurrences/bactrocera_cucurbitae/cabi_Bactrocera_cucurbitae_14Dec2020.csv</t>
-  </si>
-  <si>
-    <t>abiotic/occurrences/diaphorina_citri/diaphorinacitri_expertdata.csv</t>
-  </si>
-  <si>
-    <t>abiotic/occurrences/diaphorina_citri/cabi_diaphorina_citri_14Dec2020.csv</t>
-  </si>
-  <si>
-    <t>abiotic/occurrences/monochamus_galloprovincialis/cabi_monochamus_galloprovincialis_14Dec2020.csv</t>
-  </si>
-  <si>
-    <t>abiotic/occurrences/cicadella_viridis/cabi_cicadella_viridis_14Dec2020.csv</t>
-  </si>
-  <si>
-    <t>abiotic/occurrences/graphocephala_atropunctata/cabi_graphocephala_atropunctata_14Dec2020.csv</t>
-  </si>
-  <si>
-    <t>abiotic/occurrences/homalodisca_vitripennis/cabi_homalodisca_vitripennis_14Dec2020.csv</t>
-  </si>
-  <si>
-    <t>abiotic/occurrences/philaenus_spumarius/cabi_philaenus_spumarius_14Dec2020.csv</t>
-  </si>
-  <si>
-    <t>biotic/citrus_native_hosts_example.tif</t>
-  </si>
-  <si>
-    <t>biotic/raw_data/NVIS_5.1/aus5_1e_mvs</t>
-  </si>
-  <si>
-    <t>biotic/raw_data/NDVI/NDVI_Oct18_Mar19.grid</t>
-  </si>
-  <si>
-    <t>pathway/raw_data/Containers/postal_areas/POA_2011_AUST.gpkg</t>
-  </si>
-  <si>
-    <t>pathway/raw_data/Containers/containers_bypostcode.xls</t>
-  </si>
-  <si>
-    <t>pathway/raw_data/Ports/ports.csv</t>
-  </si>
-  <si>
-    <t>pathway/raw_data/Fertiliser/fertiliser2016_17.csv</t>
-  </si>
-  <si>
-    <t>pathway/raw_data/Fertiliser/nrm_regions/NRMR_2016_AUST.shp</t>
-  </si>
-  <si>
-    <t>pathway/raw_data/Wind/wind.gpkg</t>
-  </si>
-  <si>
-    <t>biotic/raw_data/ACLUM/clum_50m1220m.tif</t>
+    <t>Processed data directory</t>
+  </si>
+  <si>
+    <t>data/biotic/raw_data/ACLUM/clum_50m1220m.tif</t>
+  </si>
+  <si>
+    <t>data/biotic/raw_data/NVIS_5.1/aus5_1e_mvs</t>
+  </si>
+  <si>
+    <t>data/biotic/raw_data/NDVI/NDVI_Oct18_Mar19.grid</t>
+  </si>
+  <si>
+    <t>data/pathway/raw_data/Containers/postal_areas/POA_2011_AUST.gpkg</t>
+  </si>
+  <si>
+    <t>data/pathway/raw_data/Containers/containers_bypostcode.xls</t>
+  </si>
+  <si>
+    <t>data/pathway/raw_data/Ports/ports.csv</t>
+  </si>
+  <si>
+    <t>data/pathway/raw_data/Fertiliser/fertiliser2016_17.csv</t>
+  </si>
+  <si>
+    <t>data/pathway/raw_data/Fertiliser/nrm_regions/NRMR_2016_AUST.shp</t>
+  </si>
+  <si>
+    <t>data/pathway/raw_data/Wind/wind.gpkg</t>
+  </si>
+  <si>
+    <t>data/processed</t>
+  </si>
+  <si>
+    <t>Defines directory to be used to store processed datasets. Will be created (recursively) if it does not exist.</t>
+  </si>
+  <si>
+    <t>Population density data path</t>
+  </si>
+  <si>
+    <t>Raster dataset defining population density</t>
+  </si>
+  <si>
+    <t>data/pathway/raw_data/Population2016/pop_density_1000m.tif</t>
+  </si>
+  <si>
+    <t>These paths can be modified (e.g. to refer to updated datasets). However, it is the user's responsibility to ensure that the format/structure of the datasets match that of the datasets in the data repository found at https://github.com/jscamac/edmaps_data_Australia</t>
+  </si>
+  <si>
+    <t>Major airports data path</t>
+  </si>
+  <si>
+    <t>Defines distribution of tourists.</t>
+  </si>
+  <si>
+    <t>data/pathway/raw_data/Major_Airports/MajorAviationTerminals.gdb</t>
+  </si>
+  <si>
+    <t>Tourist beds data path</t>
+  </si>
+  <si>
+    <t>data/pathway/raw_data/Tourist_Beds2016/TourBedsAlbers1km.shp</t>
+  </si>
+  <si>
+    <t>data/abiotic/occurrences/gypsy_moth/cabi_Lymantria_dispar_14Dec2020.csv</t>
+  </si>
+  <si>
+    <t>data/abiotic/occurrences/apis_cerana/ApisCerana_DAWE.csv</t>
+  </si>
+  <si>
+    <t>data/abiotic/occurrences/BMSB/bmsb_presences_iprrg.csv</t>
+  </si>
+  <si>
+    <t>data/abiotic/occurrences/BMSB/cabi_halyomorpha halys_14Dec2020.csv</t>
+  </si>
+  <si>
+    <t>data/abiotic/occurrences/oriental_fruitfly/dorsalis_occurrences.csv</t>
+  </si>
+  <si>
+    <t>data/abiotic/occurrences/oriental_fruitfly/cabi_bactrocera_dorsalis_14Dec2020.csv</t>
+  </si>
+  <si>
+    <t>data/abiotic/occurrences/bactrocera_cucurbitae/cabi_Bactrocera_cucurbitae_14Dec2020.csv</t>
+  </si>
+  <si>
+    <t>data/abiotic/occurrences/diaphorina_citri/diaphorinacitri_expertdata.csv</t>
+  </si>
+  <si>
+    <t>data/abiotic/occurrences/diaphorina_citri/cabi_diaphorina_citri_14Dec2020.csv</t>
+  </si>
+  <si>
+    <t>data/abiotic/occurrences/monochamus_galloprovincialis/cabi_monochamus_galloprovincialis_14Dec2020.csv</t>
+  </si>
+  <si>
+    <t>data/abiotic/occurrences/cicadella_viridis/cabi_cicadella_viridis_14Dec2020.csv</t>
+  </si>
+  <si>
+    <t>data/abiotic/occurrences/graphocephala_atropunctata/cabi_graphocephala_atropunctata_14Dec2020.csv</t>
+  </si>
+  <si>
+    <t>data/abiotic/occurrences/homalodisca_vitripennis/cabi_homalodisca_vitripennis_14Dec2020.csv</t>
+  </si>
+  <si>
+    <t>data/abiotic/occurrences/philaenus_spumarius/cabi_philaenus_spumarius_14Dec2020.csv</t>
+  </si>
+  <si>
+    <t>data/biotic/citrus_native_hosts_example.tif</t>
   </si>
 </sst>
 </file>
@@ -1240,7 +1276,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1266,6 +1302,13 @@
       <i/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1303,7 +1346,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -1575,11 +1618,85 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1771,11 +1888,30 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="133">
+  <dxfs count="137">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2704,6 +2840,34 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE7E6E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE7E6E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE7E6E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE7E6E6"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3210,29 +3374,27 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F38E99D3-8DA3-8747-86C0-5C7DD6918E18}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34" style="21" customWidth="1"/>
     <col min="2" max="2" width="33.83203125" style="32" customWidth="1"/>
     <col min="3" max="3" width="41.5" style="21" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.83203125" style="21" customWidth="1"/>
     <col min="5" max="16384" width="10.83203125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>88</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="20"/>
     </row>
-    <row r="2" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>89</v>
       </c>
@@ -3243,7 +3405,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>92</v>
       </c>
@@ -3254,7 +3416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="34" t="s">
         <v>126</v>
       </c>
@@ -3263,7 +3425,7 @@
       </c>
       <c r="C4" s="36"/>
     </row>
-    <row r="5" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="34" t="s">
         <v>127</v>
       </c>
@@ -3272,7 +3434,7 @@
       </c>
       <c r="C5" s="36"/>
     </row>
-    <row r="6" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="34" t="s">
         <v>134</v>
       </c>
@@ -3283,7 +3445,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
         <v>163</v>
       </c>
@@ -3294,7 +3456,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="28" t="s">
         <v>94</v>
       </c>
@@ -3302,10 +3464,13 @@
         <v>95</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+        <v>256</v>
+      </c>
+      <c r="D8" s="58" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="28" t="s">
         <v>96</v>
       </c>
@@ -3313,10 +3478,11 @@
         <v>97</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+      <c r="D9" s="59"/>
+    </row>
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="28" t="s">
         <v>98</v>
       </c>
@@ -3324,10 +3490,11 @@
         <v>99</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>258</v>
+      </c>
+      <c r="D10" s="59"/>
+    </row>
+    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="28" t="s">
         <v>100</v>
       </c>
@@ -3335,10 +3502,11 @@
         <v>101</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>259</v>
+      </c>
+      <c r="D11" s="59"/>
+    </row>
+    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="28" t="s">
         <v>102</v>
       </c>
@@ -3346,10 +3514,11 @@
         <v>101</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>260</v>
+      </c>
+      <c r="D12" s="59"/>
+    </row>
+    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="28" t="s">
         <v>103</v>
       </c>
@@ -3357,10 +3526,11 @@
         <v>104</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+      <c r="D13" s="59"/>
+    </row>
+    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="28" t="s">
         <v>105</v>
       </c>
@@ -3368,10 +3538,11 @@
         <v>106</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>262</v>
+      </c>
+      <c r="D14" s="59"/>
+    </row>
+    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="28" t="s">
         <v>107</v>
       </c>
@@ -3379,10 +3550,11 @@
         <v>108</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>263</v>
+      </c>
+      <c r="D15" s="59"/>
+    </row>
+    <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="28" t="s">
         <v>230</v>
       </c>
@@ -3390,117 +3562,188 @@
         <v>231</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+        <v>264</v>
+      </c>
+      <c r="D16" s="59"/>
+    </row>
+    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="28" t="s">
+        <v>267</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>268</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>269</v>
+      </c>
+      <c r="D17" s="59"/>
+    </row>
+    <row r="18" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="28" t="s">
+        <v>271</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>272</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>273</v>
+      </c>
+      <c r="D18" s="59"/>
+    </row>
+    <row r="19" spans="1:4" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>272</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>275</v>
+      </c>
+      <c r="D19" s="60"/>
+    </row>
+    <row r="20" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A20" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B20" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="C17" s="31">
+      <c r="C20" s="31">
         <f>LN(0.5)/200</f>
         <v>-3.4657359027997266E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A18" s="28" t="s">
+    <row r="21" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A21" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="B18" s="29" t="s">
+      <c r="B21" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="C18" s="31">
+      <c r="C21" s="31">
         <f>LN(0.5)/10</f>
         <v>-6.9314718055994526E-2</v>
       </c>
     </row>
+    <row r="22" spans="1:4" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="55" t="s">
+        <v>255</v>
+      </c>
+      <c r="B22" s="56" t="s">
+        <v>266</v>
+      </c>
+      <c r="C22" s="57" t="s">
+        <v>265</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <conditionalFormatting sqref="C8">
-    <cfRule type="containsBlanks" dxfId="132" priority="14">
+  <mergeCells count="1">
+    <mergeCell ref="D8:D19"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C8 C22">
+    <cfRule type="containsBlanks" dxfId="136" priority="19">
       <formula>LEN(TRIM(C8))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="containsBlanks" dxfId="131" priority="13">
+    <cfRule type="containsBlanks" dxfId="135" priority="18">
       <formula>LEN(TRIM(C3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
+    <cfRule type="expression" dxfId="134" priority="17">
+      <formula>ISBLANK($C$10)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="expression" dxfId="133" priority="14">
+      <formula>ISBLANK($C$14)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="expression" dxfId="132" priority="13">
+      <formula>ISBLANK($C$15)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="expression" dxfId="131" priority="15">
+      <formula>ISBLANK($C$13)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
     <cfRule type="expression" dxfId="130" priority="12">
-      <formula>ISBLANK($C$10)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="129" priority="9">
-      <formula>ISBLANK($C$14)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15:C16">
-    <cfRule type="expression" dxfId="128" priority="8">
-      <formula>ISBLANK($C$15)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="127" priority="10">
-      <formula>ISBLANK($C$13)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C9">
+      <formula>ISBLANK($C$9)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="expression" dxfId="129" priority="16">
+      <formula>ISBLANK($C$12)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="expression" dxfId="128" priority="11">
+      <formula>ISBLANK($C$11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:C6">
+    <cfRule type="expression" dxfId="127" priority="8">
+      <formula>AND(NOT(ISBLANK($C$4)), ISBLANK($C$5))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4">
     <cfRule type="expression" dxfId="126" priority="7">
-      <formula>ISBLANK($C$9)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C12">
-    <cfRule type="expression" dxfId="125" priority="11">
-      <formula>ISBLANK($C$12)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="124" priority="6">
-      <formula>ISBLANK($C$11)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C5:C6">
+      <formula>AND(NOT(ISBLANK($C$5)), ISBLANK($C$4))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="expression" dxfId="125" priority="6">
+      <formula>AND(NOT(ISBLANK($C$4)), ISBLANK($C$5))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16">
+    <cfRule type="expression" dxfId="124" priority="4">
+      <formula>ISBLANK($C$16)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18">
     <cfRule type="expression" dxfId="123" priority="3">
-      <formula>AND(NOT(ISBLANK($C$4)), ISBLANK($C$5))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C4">
+      <formula>ISBLANK($C$18)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17">
     <cfRule type="expression" dxfId="122" priority="2">
-      <formula>AND(NOT(ISBLANK($C$5)), ISBLANK($C$4))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C7">
+      <formula>ISBLANK($C$17)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
     <cfRule type="expression" dxfId="121" priority="1">
-      <formula>AND(NOT(ISBLANK($C$4)), ISBLANK($C$5))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="23">
+      <formula>ISBLANK($C$19)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="28">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to container data" prompt="File path (absolute or relative to the R working directory) to the dataset giving the distribution of containers by postcode." sqref="A12:C12" xr:uid="{14B6D594-9A26-CA42-812B-5C5A86722895}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to NRM shapefile" prompt="File path (absolute or relative to the R working directory) to a polygon shapefile of NRMs (natural resource management areas)." sqref="A15 B15 C15" xr:uid="{8F72518D-BAB7-9142-9736-2536EA27E145}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to NRM shapefile" prompt="File path (absolute or relative to the R working directory) to a polygon shapefile of NRMs (natural resource management areas)." sqref="A15:C15" xr:uid="{8F72518D-BAB7-9142-9736-2536EA27E145}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to fertiliser data" prompt="File path (absolute or relative to the R working directory) to a csv containing information about fertiliser usage by NRM." sqref="A14:C14" xr:uid="{A4241D2D-0D39-E743-B011-0CB2B9A37836}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to marine ports data" prompt="File path (absolute or relative to the R working directory) to a csv containing location information for marine ports." sqref="A13:C13" xr:uid="{44AA65A2-6ACD-0941-B62C-2049F5C7A6C8}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to postal areas shapefile" prompt="File path (absolute or relative to the R working directory) to the postal areas shapefile (e.g. the path to POA_2011_AUST.shp)." sqref="A11:C11" xr:uid="{67EF961C-1766-7A4E-B6D7-223B91566EBE}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distance penalty (Torres)" prompt="Parameter controlling the distribution of Torres Strait passengers around Cairns airport._x000a__x000a_DEFAULT: LN(0.5)/10 (50% of passengers within 10km of Cairns airport)" sqref="A18:B18" xr:uid="{5FF41043-A82A-944B-945D-E8F2E51EF83B}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distance penalty (tourists)" prompt="Parameter controlling the distribution of international tourists passengers around international airport._x000a__x000a_DEFAULT: LN(0.5)/200 (50% of passengers within 200km of airport)" sqref="A17:B17" xr:uid="{33870E04-A8E1-8C4D-9B03-82E0D0B98A9C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distance penalty (Torres)" prompt="Parameter controlling the distribution of Torres Strait passengers around Cairns airport._x000a__x000a_DEFAULT: LN(0.5)/10 (50% of passengers within 10km of Cairns airport)" sqref="A21:B21" xr:uid="{5FF41043-A82A-944B-945D-E8F2E51EF83B}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Distance penalty (tourists)" prompt="Parameter controlling the distribution of international tourists passengers around international airport._x000a__x000a_DEFAULT: LN(0.5)/200 (50% of passengers within 200km of airport)" sqref="A20:B20" xr:uid="{33870E04-A8E1-8C4D-9B03-82E0D0B98A9C}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to NDVI raster" prompt="File path (absolute or relative to the R working directory) to the NDVI raster dataset. " sqref="A10:C10" xr:uid="{30D6C85A-9048-7A40-93FE-19DD2761C260}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to CLUM land use raster" prompt="File path (absolute or relative to the R working directory) to the CLUM land use raster dataset. " sqref="C8 B8 A8" xr:uid="{16AA945C-95BC-C34D-8453-8B015EFC9A02}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to CLUM land use raster" prompt="File path (absolute or relative to the R working directory) to the CLUM land use raster dataset. " sqref="A8:C8" xr:uid="{16AA945C-95BC-C34D-8453-8B015EFC9A02}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Make interactive maps?" prompt="Should interactive (html) establishment likelihood maps be produced?" sqref="A3:B3" xr:uid="{AB6F6BFD-04DD-1F47-AB62-6109D668317E}"/>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid response" error="Must be TRUE or FALSE." promptTitle="Make interactive maps?" prompt="Should interactive (html) establishment likelihood maps be produced?" sqref="C3" xr:uid="{14FD865C-56F7-6B42-A0EE-46BC6C1853BC}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid airport distance penalty" error="Must be a number less than 0." promptTitle="Distance penalty (tourists)" prompt="Parameter controlling the distribution of international tourists passengers around international airport._x000a__x000a_DEFAULT: LN(0.5)/200 (50% of passengers within 200km of airport)" sqref="C17" xr:uid="{8B7AF34B-747D-A54C-B7BD-111268DFB3AA}">
+    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid airport distance penalty" error="Must be a number less than 0." promptTitle="Distance penalty (tourists)" prompt="Parameter controlling the distribution of international tourists passengers around international airport._x000a__x000a_DEFAULT: LN(0.5)/200 (50% of passengers within 200km of airport)" sqref="C20" xr:uid="{8B7AF34B-747D-A54C-B7BD-111268DFB3AA}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid airport distance penalty" error="Must be a number less than 0." promptTitle="Distance penalty (Torres)" prompt="Parameter controlling the distribution of Torres Strait passengers around Cairns airport._x000a__x000a_DEFAULT: LN(0.5)/10 (50% of passengers within 10km of Cairns airport)" sqref="C18" xr:uid="{74A9AB0E-B263-C746-9077-ED0626B99833}">
+    <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid airport distance penalty" error="Must be a number less than 0." promptTitle="Distance penalty (Torres)" prompt="Parameter controlling the distribution of Torres Strait passengers around Cairns airport._x000a__x000a_DEFAULT: LN(0.5)/10 (50% of passengers within 10km of Cairns airport)" sqref="C21" xr:uid="{74A9AB0E-B263-C746-9077-ED0626B99833}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation showInputMessage="1" errorTitle="Invalid response" error="Must be TRUE or FALSE." promptTitle="GBIF password" prompt="GBIF password for querying the GBIF API in &quot;download&quot; mode. Go to https://www.gbif.org/ to register. Leave this blank to use GBIF's &quot;search&quot; mode." sqref="C5" xr:uid="{B0433237-8341-1A41-BC52-20A6B784A23C}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Basemap mode" prompt="Type of basemap to use for static maps. Either &quot;osm&quot; (OpenStreetMap) or &quot;boundaries&quot; (polygons)." sqref="A6 B6" xr:uid="{08117AE8-D292-1842-9E84-80BB8B707392}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Basemap mode" prompt="Type of basemap to use for static maps. Either &quot;osm&quot; (OpenStreetMap) or &quot;boundaries&quot; (polygons)." sqref="A6:B6" xr:uid="{08117AE8-D292-1842-9E84-80BB8B707392}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="GBIF password" prompt="GBIF password for querying the GBIF API in &quot;download&quot; mode. Go to https://www.gbif.org/ to register. Leave this blank to use GBIF's &quot;search&quot; mode." sqref="A5:B5" xr:uid="{AF8327F7-6AB4-254D-A562-85A05BFD02CC}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="GBIF username" prompt="GBIF username for querying the GBIF API in &quot;download&quot; mode. Go to https://www.gbif.org/ to register. Leave this blank to use GBIF's &quot;search&quot; mode." sqref="A4:B4" xr:uid="{5C32543D-BB85-AC49-99C0-4C6C3B4358FA}"/>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid response" error="Must be boundaries or osm (i.e., OpenStreetMap)" promptTitle="Basemap mode" prompt="Type of basemap to use for static maps. Either &quot;osm&quot; (OpenStreetMap) or &quot;boundaries&quot; (polygons)." sqref="C6" xr:uid="{3CC3A8BE-AB30-1148-A192-70DE8AE49742}">
@@ -3512,8 +3755,13 @@
       <formula2>1</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Minimum probability threshold" prompt="Minimum probability threshold for plotting maps. Values below this threshold will be set to zero for plotting purposes." sqref="A7:B7" xr:uid="{C15D68A0-98A0-D945-B6A6-B49C736EB3D2}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to NVIS raster" prompt="File path (absolute or relative to the R working directory) to the NVIS raster dataset. " sqref="C9 B9 A9" xr:uid="{3524C13F-E2D8-534A-BF03-893F08CA0CD9}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to Wind shapefile" prompt="File path (absolute or relative to the R working directory) to a polygon shapefile of wind speed to be associated with coastal regions." sqref="A16 B16 C16" xr:uid="{BBD5346E-86BE-7340-8C47-842D93F62CDA}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to NVIS raster" prompt="File path (absolute or relative to the R working directory) to the NVIS raster dataset. " sqref="A9:C9" xr:uid="{3524C13F-E2D8-534A-BF03-893F08CA0CD9}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to Wind shapefile" prompt="File path (absolute or relative to the R working directory) to a polygon shapefile of wind speed to be associated with coastal regions." sqref="A16:C16" xr:uid="{BBD5346E-86BE-7340-8C47-842D93F62CDA}"/>
+    <dataValidation operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Processed data directory" prompt="Directory to be used to store processed datasets. Will be created (recursively) if it does not exist." sqref="C22" xr:uid="{090147A9-F6E3-F145-829E-0B4325C48E06}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Processed data directory" prompt="Directory to be used to store processed datasets. Will be created (recursively) if it does not exist." sqref="A22:B22" xr:uid="{A64E416C-DC00-8F4F-B265-8C3CB4F65A4B}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to pop density raster" prompt="File path (absolute or relative to the R working directory) to a raster dataset of population density." sqref="B17 A17 C17" xr:uid="{97516EE7-5AE3-BA40-B4FE-30351D126FD9}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to major airports shapefile" prompt="File path (absolute or relative to the R working directory) to a vector dataset of major airports." sqref="A18 B18 C18" xr:uid="{7F766EEC-2BB4-274A-B124-AF2688D3C6BD}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to tourist beds shapefile" prompt="File path (absolute or relative to the R working directory) to a vector dataset of tourist beds." sqref="A19 B19 C19" xr:uid="{89A17CD0-617E-FA4E-BA66-7B31ECE8F76F}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3527,10 +3775,10 @@
   <dimension ref="A1:AT21"/>
   <sheetViews>
     <sheetView zoomScale="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K8" sqref="K8"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3716,7 +3964,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:46" s="41" customFormat="1" ht="35" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:46" s="41" customFormat="1" ht="69" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
@@ -3738,7 +3986,7 @@
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="11" t="s">
-        <v>269</v>
+        <v>290</v>
       </c>
       <c r="J2" s="9"/>
       <c r="K2" s="8"/>
@@ -3825,7 +4073,7 @@
       </c>
       <c r="M3" s="12"/>
       <c r="N3" s="12" t="s">
-        <v>255</v>
+        <v>276</v>
       </c>
       <c r="O3" s="11"/>
       <c r="P3" s="11"/>
@@ -3992,7 +4240,7 @@
       <c r="K5" s="12"/>
       <c r="L5" s="13"/>
       <c r="M5" s="12" t="s">
-        <v>256</v>
+        <v>277</v>
       </c>
       <c r="N5" s="12"/>
       <c r="O5" s="11"/>
@@ -4075,10 +4323,10 @@
       <c r="K6" s="12"/>
       <c r="L6" s="13"/>
       <c r="M6" s="12" t="s">
-        <v>257</v>
+        <v>278</v>
       </c>
       <c r="N6" s="12" t="s">
-        <v>258</v>
+        <v>279</v>
       </c>
       <c r="O6" s="11"/>
       <c r="P6" s="11"/>
@@ -4158,7 +4406,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>269</v>
+        <v>290</v>
       </c>
       <c r="M7" s="12"/>
       <c r="N7" s="12"/>
@@ -4210,7 +4458,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>269</v>
+        <v>290</v>
       </c>
       <c r="K8" s="12" t="s">
         <v>71</v>
@@ -4219,10 +4467,10 @@
         <v>1970</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>259</v>
+        <v>280</v>
       </c>
       <c r="N8" s="12" t="s">
-        <v>260</v>
+        <v>281</v>
       </c>
       <c r="R8" s="12" t="s">
         <v>189</v>
@@ -4258,7 +4506,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="9" spans="1:46" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:46" ht="68" x14ac:dyDescent="0.2">
       <c r="A9" s="45" t="s">
         <v>242</v>
       </c>
@@ -4278,7 +4526,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>269</v>
+        <v>290</v>
       </c>
       <c r="N9" s="12"/>
       <c r="R9" s="12" t="s">
@@ -4335,7 +4583,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>269</v>
+        <v>290</v>
       </c>
       <c r="K10" s="12" t="s">
         <v>133</v>
@@ -4345,7 +4593,7 @@
       </c>
       <c r="M10" s="12"/>
       <c r="N10" s="12" t="s">
-        <v>261</v>
+        <v>282</v>
       </c>
       <c r="R10" s="12" t="s">
         <v>189</v>
@@ -4404,7 +4652,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>269</v>
+        <v>290</v>
       </c>
       <c r="K11" s="12" t="s">
         <v>80</v>
@@ -4413,10 +4661,10 @@
         <v>1970</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>262</v>
+        <v>283</v>
       </c>
       <c r="N11" s="12" t="s">
-        <v>263</v>
+        <v>284</v>
       </c>
       <c r="P11" s="54">
         <v>100000</v>
@@ -4449,7 +4697,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="12" spans="1:46" ht="51" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:46" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="45" t="s">
         <v>251</v>
       </c>
@@ -4471,9 +4719,7 @@
       <c r="G12" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="I12" s="11" t="s">
-        <v>269</v>
-      </c>
+      <c r="I12" s="11"/>
       <c r="M12" s="12"/>
       <c r="N12" s="12"/>
       <c r="T12" s="12" t="s">
@@ -4620,7 +4866,7 @@
       </c>
       <c r="M15" s="12"/>
       <c r="N15" s="12" t="s">
-        <v>264</v>
+        <v>285</v>
       </c>
       <c r="T15" s="12" t="s">
         <v>206</v>
@@ -4675,7 +4921,7 @@
       </c>
       <c r="M16" s="12"/>
       <c r="N16" s="12" t="s">
-        <v>265</v>
+        <v>286</v>
       </c>
       <c r="Q16" s="14">
         <f t="shared" ref="Q16" si="0">LN(0.5)/1</f>
@@ -4734,7 +4980,7 @@
       </c>
       <c r="M17" s="12"/>
       <c r="N17" s="12" t="s">
-        <v>266</v>
+        <v>287</v>
       </c>
       <c r="Q17" s="14">
         <f>LN(0.5)/1</f>
@@ -4793,7 +5039,7 @@
       </c>
       <c r="M18" s="12"/>
       <c r="N18" s="12" t="s">
-        <v>267</v>
+        <v>288</v>
       </c>
       <c r="Q18" s="14">
         <f t="shared" ref="Q18" si="1">LN(0.5)/1</f>
@@ -4852,7 +5098,7 @@
       </c>
       <c r="M19" s="12"/>
       <c r="N19" s="12" t="s">
-        <v>268</v>
+        <v>289</v>
       </c>
       <c r="Q19" s="14">
         <f>LN(0.5)/1</f>
@@ -4944,7 +5190,7 @@
       <c r="K21" s="12"/>
       <c r="L21" s="13"/>
       <c r="M21" s="12" t="s">
-        <v>256</v>
+        <v>277</v>
       </c>
       <c r="N21" s="40"/>
       <c r="O21" s="17"/>

</xml_diff>